<commit_message>
Added get products sku
</commit_message>
<xml_diff>
--- a/data/products-temp.xlsx
+++ b/data/products-temp.xlsx
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,6 +1226,15 @@
       <c r="E3">
         <v>49313</v>
       </c>
+      <c r="F3">
+        <v>49313</v>
+      </c>
+      <c r="G3">
+        <v>49313</v>
+      </c>
+      <c r="H3">
+        <v>49313</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
Progress on converting fences into actual product
</commit_message>
<xml_diff>
--- a/data/products-temp.xlsx
+++ b/data/products-temp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\html\fc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/fencing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39490857-1D89-DB4F-B806-2026BFF3CADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23820" windowHeight="11745"/>
+    <workbookView xWindow="-37260" yWindow="-360" windowWidth="36060" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -291,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1139,26 +1140,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>49922</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>49313</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1340,7 +1341,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>49925</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>52</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>49943</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>49928</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1516,7 +1517,7 @@
         <v>49949</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>49934</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>49952</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>77</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>49830</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1643,7 +1644,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
added condition for raked_post
</commit_message>
<xml_diff>
--- a/data/products-temp.xlsx
+++ b/data/products-temp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/fencing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39490857-1D89-DB4F-B806-2026BFF3CADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D9D123-9D13-124A-8A9B-BC696DAD6505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37260" yWindow="-360" windowWidth="36060" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40140" yWindow="-5300" windowWidth="39720" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -437,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +638,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +808,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -820,6 +826,7 @@
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1143,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1186,7 +1193,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1212,7 +1219,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1238,7 +1245,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1264,7 +1271,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1290,7 +1297,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1316,7 +1323,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1342,7 +1349,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1368,7 +1375,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1394,7 +1401,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1440,7 +1447,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1466,7 +1473,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1492,7 +1499,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1518,7 +1525,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1619,7 +1626,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="2" t="s">

</xml_diff>